<commit_message>
ajuste da planilha de calculo
</commit_message>
<xml_diff>
--- a/src/Atividade Linguagem de Programação.xlsx
+++ b/src/Atividade Linguagem de Programação.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\fag\fatec\2 semestre\linguagem de programação\E1\E1_Fagner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B8D7FD9-391B-4737-9302-16914DFD92A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2668B3C8-CDA2-4398-8530-3EE2B367854A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{6F3C35B3-66BF-4733-BD21-4347552E10B4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="1" xr2:uid="{6F3C35B3-66BF-4733-BD21-4347552E10B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Calculo de média" sheetId="1" r:id="rId1"/>
     <sheet name="MÚSICA" sheetId="2" r:id="rId2"/>
     <sheet name="DOODLE" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,6 +29,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -38,6 +40,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
+    <t>Aluno</t>
+  </si>
+  <si>
     <t>Nota P1</t>
   </si>
   <si>
@@ -59,100 +64,97 @@
     <t>MÉDIA</t>
   </si>
   <si>
+    <t>Aluno1</t>
+  </si>
+  <si>
+    <t>Aluno2</t>
+  </si>
+  <si>
+    <t>Aluno3</t>
+  </si>
+  <si>
+    <t>Aluno4</t>
+  </si>
+  <si>
+    <t>Aluno5</t>
+  </si>
+  <si>
+    <t>Aluno6</t>
+  </si>
+  <si>
+    <t>Aluno7</t>
+  </si>
+  <si>
+    <t>Aluno8</t>
+  </si>
+  <si>
+    <t>Aluno9</t>
+  </si>
+  <si>
+    <t>Aluno10</t>
+  </si>
+  <si>
+    <t>MÚSICA - FAROESTE CABOCLO</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
     <t>Personagem</t>
   </si>
   <si>
+    <t>Arma</t>
+  </si>
+  <si>
+    <t>Cidade</t>
+  </si>
+  <si>
     <t>- nome: String</t>
   </si>
   <si>
+    <t>- modelo: String</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - String nome</t>
+  </si>
+  <si>
     <t>- origem: String</t>
   </si>
   <si>
+    <t>- municaoAtual: Integer</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - String regiao</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - estaVivo: Boolean</t>
+  </si>
+  <si>
+    <t>- capacidadeMunicao: Integer</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Boolean eViolenta</t>
+  </si>
+  <si>
+    <t>- dono: Personagem</t>
+  </si>
+  <si>
+    <t>+ atirar(): Boolean</t>
+  </si>
+  <si>
     <t>+ viajar(destino: String): void</t>
   </si>
   <si>
-    <t>Arma</t>
-  </si>
-  <si>
-    <t>- modelo: String</t>
-  </si>
-  <si>
-    <t>- municaoAtual: Integer</t>
-  </si>
-  <si>
-    <t>- capacidadeMunicao: Integer</t>
-  </si>
-  <si>
-    <t>- dono: Personagem</t>
-  </si>
-  <si>
-    <t>+ atirar(): Boolean</t>
-  </si>
-  <si>
     <t>+ recarregar(quantidade: Integer): void</t>
   </si>
   <si>
-    <t>MÚSICA - FAROESTE CABOCLO</t>
-  </si>
-  <si>
-    <t>Aluno</t>
-  </si>
-  <si>
-    <t>Aluno1</t>
-  </si>
-  <si>
-    <t>Aluno2</t>
-  </si>
-  <si>
-    <t>Aluno3</t>
-  </si>
-  <si>
-    <t>Aluno4</t>
-  </si>
-  <si>
-    <t>Aluno5</t>
-  </si>
-  <si>
-    <t>Aluno6</t>
-  </si>
-  <si>
-    <t>Aluno7</t>
-  </si>
-  <si>
-    <t>Aluno8</t>
-  </si>
-  <si>
-    <t>Aluno9</t>
-  </si>
-  <si>
-    <t>Aluno10</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - estaVivo: Boolean</t>
+    <t xml:space="preserve"> + transformar(cidade: String) void</t>
   </si>
   <si>
     <t>Objeto: joaoDeSantoCristo</t>
   </si>
   <si>
     <t>Objeto: winchester22</t>
-  </si>
-  <si>
-    <t>Cidade</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - String nome</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - String regiao</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - Boolean eViolenta</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> + transformar(cidade: String) void</t>
   </si>
   <si>
     <t>Objeto: brasilia</t>
@@ -162,7 +164,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -608,6 +610,13 @@
       </border>
     </dxf>
     <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -625,13 +634,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <fill>
@@ -666,7 +668,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2844FB43-C45D-4F6A-8B49-E51137E714C5}" name="Tabela1" displayName="Tabela1" ref="B1:H11" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2844FB43-C45D-4F6A-8B49-E51137E714C5}" name="Tabela1" displayName="Tabela1" ref="B1:H11" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10" headerRowBorderDxfId="8" tableBorderDxfId="9" totalsRowBorderDxfId="7">
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{DDA608E6-1C98-4DA4-BB2B-756554180B84}" name="Nota P1" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{32B819E0-5504-431B-B275-A517B2CAE17C}" name="Nota E1" dataDxfId="5"/>
@@ -683,9 +685,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -723,7 +725,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -829,7 +831,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -971,7 +973,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -982,10 +984,10 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="4" width="9.42578125" customWidth="1"/>
     <col min="5" max="5" width="10.140625" customWidth="1"/>
@@ -993,35 +995,35 @@
     <col min="8" max="8" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="12" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1">
         <v>5</v>
@@ -1046,9 +1048,9 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1">
         <v>5</v>
@@ -1073,9 +1075,9 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1">
         <v>10</v>
@@ -1100,9 +1102,9 @@
         <v>11.25</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1">
         <v>10</v>
@@ -1127,9 +1129,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="B6" s="1">
         <v>6</v>
@@ -1154,9 +1156,9 @@
         <v>6.55</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1">
         <v>6</v>
@@ -1174,16 +1176,16 @@
         <v>0</v>
       </c>
       <c r="G7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" s="3">
         <f t="shared" si="0"/>
-        <v>7.45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>7.95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="B8" s="1">
         <v>9</v>
@@ -1208,9 +1210,9 @@
         <v>7.55</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="B9" s="1">
         <v>8</v>
@@ -1235,9 +1237,9 @@
         <v>7.9</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="B10" s="1">
         <v>5</v>
@@ -1262,9 +1264,9 @@
         <v>7.3999999999999995</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="B11" s="1">
         <v>4</v>
@@ -1307,15 +1309,15 @@
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="39.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="36.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="60.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:6" ht="15.75" thickBot="1"/>
+    <row r="2" spans="2:6" ht="15.75" thickBot="1">
       <c r="B2" s="15" t="s">
         <v>18</v>
       </c>
@@ -1324,94 +1326,94 @@
       <c r="E2" s="16"/>
       <c r="F2" s="17"/>
     </row>
-    <row r="3" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" ht="15.75" thickBot="1">
       <c r="F3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="15.75" thickBot="1">
       <c r="B4" s="6" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6">
       <c r="B5" s="7" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6">
       <c r="B6" s="8" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6">
       <c r="B7" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="8" t="s">
-        <v>14</v>
-      </c>
       <c r="F7" s="8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="15.75" thickBot="1">
       <c r="B8" s="8"/>
       <c r="D8" s="9" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="F8" s="8"/>
     </row>
-    <row r="9" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" ht="15.75" thickBot="1">
       <c r="B9" s="9"/>
       <c r="D9" s="7" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="F9" s="9"/>
     </row>
-    <row r="10" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6" ht="15.75" thickBot="1">
       <c r="B10" s="7" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6">
       <c r="B11" s="8"/>
       <c r="F11" s="8"/>
     </row>
-    <row r="12" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:6" ht="15.75" thickBot="1">
       <c r="B12" s="9"/>
       <c r="F12" s="9"/>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6">
       <c r="B14" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D14" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="F14" t="s">
         <v>39</v>
@@ -1434,7 +1436,7 @@
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
Inserção de calculo de média e criação de um menu interativo via terminal para selecionar as opções existentes
</commit_message>
<xml_diff>
--- a/src/Atividade Linguagem de Programação.xlsx
+++ b/src/Atividade Linguagem de Programação.xlsx
@@ -1,21 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\fag\fatec\2 semestre\linguagem de programação\E1\E1_Fagner\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\fag\dev\LP\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2668B3C8-CDA2-4398-8530-3EE2B367854A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78A8CED3-3BEE-4426-8FE8-CE127A822BDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="1" xr2:uid="{6F3C35B3-66BF-4733-BD21-4347552E10B4}"/>
+    <workbookView xWindow="348" yWindow="2628" windowWidth="17280" windowHeight="8880" xr2:uid="{6F3C35B3-66BF-4733-BD21-4347552E10B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Calculo de média" sheetId="1" r:id="rId1"/>
-    <sheet name="MÚSICA" sheetId="2" r:id="rId2"/>
-    <sheet name="DOODLE" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -29,16 +27,17 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Aluno</t>
   </si>
@@ -92,88 +91,14 @@
   </si>
   <si>
     <t>Aluno10</t>
-  </si>
-  <si>
-    <t>MÚSICA - FAROESTE CABOCLO</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Personagem</t>
-  </si>
-  <si>
-    <t>Arma</t>
-  </si>
-  <si>
-    <t>Cidade</t>
-  </si>
-  <si>
-    <t>- nome: String</t>
-  </si>
-  <si>
-    <t>- modelo: String</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - String nome</t>
-  </si>
-  <si>
-    <t>- origem: String</t>
-  </si>
-  <si>
-    <t>- municaoAtual: Integer</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - String regiao</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - estaVivo: Boolean</t>
-  </si>
-  <si>
-    <t>- capacidadeMunicao: Integer</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - Boolean eViolenta</t>
-  </si>
-  <si>
-    <t>- dono: Personagem</t>
-  </si>
-  <si>
-    <t>+ atirar(): Boolean</t>
-  </si>
-  <si>
-    <t>+ viajar(destino: String): void</t>
-  </si>
-  <si>
-    <t>+ recarregar(quantidade: Integer): void</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> + transformar(cidade: String) void</t>
-  </si>
-  <si>
-    <t>Objeto: joaoDeSantoCristo</t>
-  </si>
-  <si>
-    <t>Objeto: winchester22</t>
-  </si>
-  <si>
-    <t>Objeto: brasilia</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -209,7 +134,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -306,100 +231,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -416,32 +252,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -610,13 +430,6 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -634,6 +447,13 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <fill>
@@ -668,7 +488,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2844FB43-C45D-4F6A-8B49-E51137E714C5}" name="Tabela1" displayName="Tabela1" ref="B1:H11" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10" headerRowBorderDxfId="8" tableBorderDxfId="9" totalsRowBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2844FB43-C45D-4F6A-8B49-E51137E714C5}" name="Tabela1" displayName="Tabela1" ref="B1:H11" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{DDA608E6-1C98-4DA4-BB2B-756554180B84}" name="Nota P1" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{32B819E0-5504-431B-B275-A517B2CAE17C}" name="Nota E1" dataDxfId="5"/>
@@ -685,7 +505,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -983,45 +803,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4334EAF-FEE7-4606-BFB3-1138F905AC68}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="4" width="9.42578125" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" customWidth="1"/>
-    <col min="8" max="8" width="25.7109375" customWidth="1"/>
+    <col min="2" max="4" width="9.44140625" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" customWidth="1"/>
+    <col min="8" max="8" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="11" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="14" t="s">
+      <c r="G1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1048,7 +868,7 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -1075,7 +895,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -1092,17 +912,17 @@
         <v>10</v>
       </c>
       <c r="F4" s="2">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G4" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4" s="3">
         <f>_xlfn.LET(_xlpm.nota_base,(B4*0.5+C4*0.2+D4*0.3+G4+F4*0.15),(_xlpm.nota_base*0.5)+(IF(_xlpm.nota_base&gt;5.9,1,0)*E4*0.5))</f>
-        <v>11.25</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -1129,7 +949,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -1156,7 +976,7 @@
         <v>6.55</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -1183,7 +1003,7 @@
         <v>7.95</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -1210,7 +1030,7 @@
         <v>7.55</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
@@ -1237,7 +1057,7 @@
         <v>7.9</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
@@ -1264,7 +1084,7 @@
         <v>7.3999999999999995</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
@@ -1292,152 +1112,11 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D643D501-C0CA-4972-BF57-4423101D274E}">
-  <dimension ref="B1:F14"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="2" width="39.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="60.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:6" ht="15.75" thickBot="1"/>
-    <row r="2" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B2" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="17"/>
-    </row>
-    <row r="3" spans="2:6" ht="15.75" thickBot="1">
-      <c r="F3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B4" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6">
-      <c r="B5" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6">
-      <c r="B6" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6">
-      <c r="B7" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B8" s="8"/>
-      <c r="D8" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8" s="8"/>
-    </row>
-    <row r="9" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B9" s="9"/>
-      <c r="D9" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F9" s="9"/>
-    </row>
-    <row r="10" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B10" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6">
-      <c r="B11" s="8"/>
-      <c r="F11" s="8"/>
-    </row>
-    <row r="12" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B12" s="9"/>
-      <c r="F12" s="9"/>
-    </row>
-    <row r="14" spans="2:6">
-      <c r="B14" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" t="s">
-        <v>38</v>
-      </c>
-      <c r="F14" t="s">
-        <v>39</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B2:F2"/>
-  </mergeCells>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50BB5790-7176-4609-B324-1147FCF52ABF}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
 </file>
</xml_diff>